<commit_message>
Crane Bay Box 1 Build
</commit_message>
<xml_diff>
--- a/Config/Calibrations/CraneBayOneBoxCalibration.xlsx
+++ b/Config/Calibrations/CraneBayOneBoxCalibration.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="15195" windowHeight="13035"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="15195" windowHeight="13035" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Displacement Cal" sheetId="1" r:id="rId1"/>
+    <sheet name="Shunt Cal" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="22">
   <si>
     <t>Command</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Load Cell Offset</t>
+  </si>
+  <si>
+    <t>Load Cell - Shunt Calibration</t>
+  </si>
+  <si>
+    <t>11/23/2010 - Large Scale LBCB 3</t>
+  </si>
+  <si>
+    <t>Ray, Michael, Alan, Ken, Party in the Crane Bay</t>
   </si>
 </sst>
 </file>
@@ -491,7 +500,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$30:$C$42</c:f>
+              <c:f>'Displacement Cal'!$C$30:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -539,7 +548,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$30:$E$42</c:f>
+              <c:f>'Displacement Cal'!$E$30:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -930,7 +939,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$52:$D$64</c:f>
+              <c:f>'Displacement Cal'!$D$52:$D$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -978,7 +987,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$52:$E$64</c:f>
+              <c:f>'Displacement Cal'!$E$52:$E$64</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1422,7 +1431,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$114:$D$122</c:f>
+              <c:f>'Displacement Cal'!$D$114:$D$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1458,7 +1467,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$114:$E$122</c:f>
+              <c:f>'Displacement Cal'!$E$114:$E$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1837,7 +1846,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$11:$D$21</c:f>
+              <c:f>'Displacement Cal'!$D$11:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1879,7 +1888,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$11:$E$21</c:f>
+              <c:f>'Displacement Cal'!$E$11:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2264,7 +2273,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$11:$C$21</c:f>
+              <c:f>'Displacement Cal'!$C$11:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2306,7 +2315,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$11:$E$21</c:f>
+              <c:f>'Displacement Cal'!$E$11:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2691,7 +2700,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$75:$C$85</c:f>
+              <c:f>'Displacement Cal'!$C$75:$C$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2733,7 +2742,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$75:$E$85</c:f>
+              <c:f>'Displacement Cal'!$E$75:$E$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3118,7 +3127,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$95:$C$106</c:f>
+              <c:f>'Displacement Cal'!$C$95:$C$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3163,7 +3172,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$95:$E$106</c:f>
+              <c:f>'Displacement Cal'!$E$95:$E$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3551,7 +3560,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$52:$C$64</c:f>
+              <c:f>'Displacement Cal'!$C$52:$C$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3599,7 +3608,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$52:$E$64</c:f>
+              <c:f>'Displacement Cal'!$E$52:$E$64</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3990,7 +3999,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$114:$C$122</c:f>
+              <c:f>'Displacement Cal'!$C$114:$C$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -4026,7 +4035,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$114:$E$123</c:f>
+              <c:f>'Displacement Cal'!$E$114:$E$123</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4413,7 +4422,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$30:$D$42</c:f>
+              <c:f>'Displacement Cal'!$D$30:$D$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4461,7 +4470,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$30:$E$42</c:f>
+              <c:f>'Displacement Cal'!$E$30:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4852,7 +4861,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$75:$D$85</c:f>
+              <c:f>'Displacement Cal'!$D$75:$D$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4894,7 +4903,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$75:$E$85</c:f>
+              <c:f>'Displacement Cal'!$E$75:$E$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5279,7 +5288,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$95:$D$106</c:f>
+              <c:f>'Displacement Cal'!$D$95:$D$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5324,7 +5333,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1'!$E$95:$E$106</c:f>
+              <c:f>'Displacement Cal'!$E$95:$E$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -6259,8 +6268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A122" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7696,12 +7705,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18">
+      <c r="A5" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18">
+      <c r="A10" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18">
+      <c r="A14" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18">
+      <c r="A18" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18">
+      <c r="A22" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18">
+      <c r="A26" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Displacement Testing One box crane bay
</commit_message>
<xml_diff>
--- a/Config/Calibrations/CraneBayOneBoxCalibration.xlsx
+++ b/Config/Calibrations/CraneBayOneBoxCalibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="15195" windowHeight="13035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="15195" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="Displacement Cal" sheetId="1" r:id="rId1"/>
@@ -1341,85 +1341,14 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.44328182054166304"/>
-                  <c:y val="0.22368411718805417"/>
+                  <c:x val="-0.38730674422299977"/>
+                  <c:y val="0.21085675548834543"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                        <a:solidFill>
-                          <a:srgbClr val="000000"/>
-                        </a:solidFill>
-                        <a:latin typeface="Arial"/>
-                        <a:ea typeface="Arial"/>
-                        <a:cs typeface="Arial"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                        <a:solidFill>
-                          <a:srgbClr val="000000"/>
-                        </a:solidFill>
-                        <a:latin typeface="Arial"/>
-                        <a:cs typeface="Arial"/>
-                      </a:rPr>
-                      <a:t>y = 0.9714x + 12.822</a:t>
-                    </a:r>
-                  </a:p>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                        <a:solidFill>
-                          <a:srgbClr val="000000"/>
-                        </a:solidFill>
-                        <a:latin typeface="Arial"/>
-                        <a:ea typeface="Arial"/>
-                        <a:cs typeface="Arial"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                        <a:solidFill>
-                          <a:srgbClr val="000000"/>
-                        </a:solidFill>
-                        <a:latin typeface="Arial"/>
-                        <a:cs typeface="Arial"/>
-                      </a:rPr>
-                      <a:t>R</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000">
-                        <a:solidFill>
-                          <a:srgbClr val="000000"/>
-                        </a:solidFill>
-                        <a:latin typeface="Arial"/>
-                        <a:cs typeface="Arial"/>
-                      </a:rPr>
-                      <a:t>2</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                        <a:solidFill>
-                          <a:srgbClr val="000000"/>
-                        </a:solidFill>
-                        <a:latin typeface="Arial"/>
-                        <a:cs typeface="Arial"/>
-                      </a:rPr>
-                      <a:t> = 1</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1427,6 +1356,23 @@
                   <a:noFill/>
                 </a:ln>
               </c:spPr>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                      <a:ea typeface="Arial"/>
+                      <a:cs typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -6268,8 +6214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A122"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7707,7 +7653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>